<commit_message>
Further localization preparation work
</commit_message>
<xml_diff>
--- a/stm-unity/Assets/Localization/Sports Team Manager Localization.xlsx
+++ b/stm-unity/Assets/Localization/Sports Team Manager Localization.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="190">
   <si>
     <t>key</t>
   </si>
@@ -35,6 +35,12 @@
   </si>
   <si>
     <t>Body</t>
+  </si>
+  <si>
+    <t>BOWMAN</t>
+  </si>
+  <si>
+    <t>Bowman</t>
   </si>
   <si>
     <t>CHARISMA</t>
@@ -97,6 +103,18 @@
     <t>Ideal Placements</t>
   </si>
   <si>
+    <t>GRINDER</t>
+  </si>
+  <si>
+    <t>Grinder</t>
+  </si>
+  <si>
+    <t>HELMSMAN</t>
+  </si>
+  <si>
+    <t>Helmsman</t>
+  </si>
+  <si>
     <t>HELP</t>
   </si>
   <si>
@@ -157,6 +175,12 @@
     <t>What do you want to ask?</t>
   </si>
   <si>
+    <t>MIDBOWMAN</t>
+  </si>
+  <si>
+    <t>Mid-Bowman</t>
+  </si>
+  <si>
     <t>MOOD</t>
   </si>
   <si>
@@ -167,6 +191,12 @@
   </si>
   <si>
     <t>Name:</t>
+  </si>
+  <si>
+    <t>NAVIGATOR</t>
+  </si>
+  <si>
+    <t>Navigator</t>
   </si>
   <si>
     <t>NEW_GAME</t>
@@ -188,6 +218,12 @@
   </si>
   <si>
     <t>Perception</t>
+  </si>
+  <si>
+    <t>PITMAN</t>
+  </si>
+  <si>
+    <t>Pitman</t>
   </si>
   <si>
     <t>POSITION_NAME</t>
@@ -268,6 +304,12 @@
     <t>Skills Required</t>
   </si>
   <si>
+    <t>SKIPPER</t>
+  </si>
+  <si>
+    <t>Skipper</t>
+  </si>
+  <si>
     <t>TALK_TIME_REMAINING</t>
   </si>
   <si>
@@ -290,6 +332,12 @@
   </si>
   <si>
     <t>Team Name:</t>
+  </si>
+  <si>
+    <t>TRIMMER</t>
+  </si>
+  <si>
+    <t>Trimmer</t>
   </si>
   <si>
     <t>WILLPOWER</t>
@@ -316,52 +364,225 @@
     <t>Yes</t>
   </si>
   <si>
-    <t>SKIPPER</t>
+    <t>CANCEL</t>
   </si>
   <si>
-    <t>Skipper</t>
+    <t>Cancel</t>
   </si>
   <si>
-    <t>HELMSMAN</t>
+    <t>NEW_GAME_OVERWRITE</t>
   </si>
   <si>
-    <t>Helmsman</t>
+    <t>A game with this team name already exists!
+Are you sure you want to create a new game and overwrite the existing game?</t>
   </si>
   <si>
-    <t>MIDBOWMAN</t>
+    <t>OVERWRITE</t>
   </si>
   <si>
-    <t>Mid-Bowman</t>
+    <t>Overwrite</t>
   </si>
   <si>
-    <t>NAVIGATOR</t>
+    <t>NEW_GAME_CREATION_ERROR</t>
   </si>
   <si>
-    <t>Navigator</t>
+    <t>Game not created. Please try again.</t>
   </si>
   <si>
-    <t>PITMAN</t>
+    <t>LOAD_GAME_MISSING_FILES</t>
   </si>
   <si>
-    <t>Pitman</t>
+    <t>Unable to load game due to missing files. Please try loading a different game.</t>
   </si>
   <si>
-    <t>TRIMMER</t>
+    <t>LOAD_GAME_NOT_LOADED</t>
   </si>
   <si>
-    <t>Trimmer</t>
+    <t>Game was not loaded. Please try again.</t>
   </si>
   <si>
-    <t>GRINDER</t>
+    <t>NO_ROLE</t>
   </si>
   <si>
-    <t>Grinder</t>
+    <t>No Role</t>
   </si>
   <si>
-    <t>BOWMAN</t>
+    <t>MEETING_INTRO</t>
   </si>
   <si>
-    <t>Bowman</t>
+    <t>You wanted to see me?</t>
+  </si>
+  <si>
+    <t>MEETING_EARLY_EXIT</t>
+  </si>
+  <si>
+    <t>Nevermind, goodbye.</t>
+  </si>
+  <si>
+    <t>MEETING_EXIT</t>
+  </si>
+  <si>
+    <t>OK&lt; thank you for telling me that.</t>
+  </si>
+  <si>
+    <t>RECRUITMENT_INTRO</t>
+  </si>
+  <si>
+    <t>Your recruits are here. What do you want to ask them all or who do you want to hire?</t>
+  </si>
+  <si>
+    <t>HIRE_WARNING_POSSIBLE</t>
+  </si>
+  <si>
+    <t>Are you sure you want to hire {0}?</t>
+  </si>
+  <si>
+    <t>x{0}</t>
+  </si>
+  <si>
+    <t>HIRE_WARNING_NOT_POSSIBLE</t>
+  </si>
+  <si>
+    <t>You don't have enough time left to hire this person.</t>
+  </si>
+  <si>
+    <t>RECRUIT_GREETING_0</t>
+  </si>
+  <si>
+    <t>Hello</t>
+  </si>
+  <si>
+    <t>RECRUIT_GREETING_1</t>
+  </si>
+  <si>
+    <t>Hey</t>
+  </si>
+  <si>
+    <t>RECRUIT_GREETING_2</t>
+  </si>
+  <si>
+    <t>Hi</t>
+  </si>
+  <si>
+    <t>RECRUIT_GREETING_3</t>
+  </si>
+  <si>
+    <t>Hey there</t>
+  </si>
+  <si>
+    <t>EXCLAIMATION_MARK</t>
+  </si>
+  <si>
+    <t>!</t>
+  </si>
+  <si>
+    <t>AMPERSAND</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> &amp; </t>
+  </si>
+  <si>
+    <t>RACE_BUTTON_PRACTICE</t>
+  </si>
+  <si>
+    <t>Practice {0}/{1}</t>
+  </si>
+  <si>
+    <t>x{0}{1}</t>
+  </si>
+  <si>
+    <t>RACE_BUTTON_RACE</t>
+  </si>
+  <si>
+    <t>Race!</t>
+  </si>
+  <si>
+    <t>RACE_CONFIRM_ALLOWANCE_REMAINING</t>
+  </si>
+  <si>
+    <t>You have {0} Talk Time remaining! If you don't use it before the race, they will be lost.
+Are you sure you want to race with this line-up now?</t>
+  </si>
+  <si>
+    <t>RACE_CONFIRM_NO_ALLOWANCE</t>
+  </si>
+  <si>
+    <t>Are you sure you want to race with this line-up now?</t>
+  </si>
+  <si>
+    <t>POSITION_1</t>
+  </si>
+  <si>
+    <t>1st</t>
+  </si>
+  <si>
+    <t>POSITION_2</t>
+  </si>
+  <si>
+    <t>2nd</t>
+  </si>
+  <si>
+    <t>POSITION_3</t>
+  </si>
+  <si>
+    <t>3rd</t>
+  </si>
+  <si>
+    <t>POSITION_4</t>
+  </si>
+  <si>
+    <t>4th</t>
+  </si>
+  <si>
+    <t>POSITION_5</t>
+  </si>
+  <si>
+    <t>5th</t>
+  </si>
+  <si>
+    <t>POSITION_6</t>
+  </si>
+  <si>
+    <t>6th</t>
+  </si>
+  <si>
+    <t>POSITION_7</t>
+  </si>
+  <si>
+    <t>7th</t>
+  </si>
+  <si>
+    <t>POSITION_8</t>
+  </si>
+  <si>
+    <t>8th</t>
+  </si>
+  <si>
+    <t>POSITION_9</t>
+  </si>
+  <si>
+    <t>9th</t>
+  </si>
+  <si>
+    <t>POSITION_10</t>
+  </si>
+  <si>
+    <t>10th</t>
+  </si>
+  <si>
+    <t>RACE_POSITION</t>
+  </si>
+  <si>
+    <t>Position:</t>
+  </si>
+  <si>
+    <t>RACE_RESULT_POSTION</t>
+  </si>
+  <si>
+    <t>{0} finished {1}!</t>
+  </si>
+  <si>
+    <t>{0}x{1}!</t>
   </si>
 </sst>
 </file>
@@ -376,12 +597,18 @@
     </font>
     <font/>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -395,7 +622,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
@@ -407,6 +634,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -532,17 +762,17 @@
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
-      <c r="N4" s="1"/>
-      <c r="O4" s="1"/>
-      <c r="P4" s="1"/>
-      <c r="Q4" s="1"/>
-      <c r="R4" s="1"/>
-      <c r="S4" s="1"/>
-      <c r="T4" s="1"/>
-      <c r="U4" s="1"/>
-      <c r="V4" s="1"/>
-      <c r="W4" s="1"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="3"/>
+      <c r="U4" s="3"/>
+      <c r="V4" s="3"/>
+      <c r="W4" s="3"/>
     </row>
     <row r="5" ht="14.25" customHeight="1">
       <c r="A5" s="2" t="s">
@@ -559,17 +789,17 @@
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
-      <c r="M5" s="3"/>
-      <c r="N5" s="3"/>
-      <c r="O5" s="3"/>
-      <c r="P5" s="3"/>
-      <c r="Q5" s="3"/>
-      <c r="R5" s="3"/>
-      <c r="S5" s="3"/>
-      <c r="T5" s="3"/>
-      <c r="U5" s="3"/>
-      <c r="V5" s="3"/>
-      <c r="W5" s="3"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="1"/>
+      <c r="S5" s="1"/>
+      <c r="T5" s="1"/>
+      <c r="U5" s="1"/>
+      <c r="V5" s="1"/>
+      <c r="W5" s="1"/>
     </row>
     <row r="6" ht="14.25" customHeight="1">
       <c r="A6" s="2" t="s">
@@ -586,17 +816,17 @@
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
-      <c r="N6" s="1"/>
-      <c r="O6" s="1"/>
-      <c r="P6" s="1"/>
-      <c r="Q6" s="1"/>
-      <c r="R6" s="1"/>
-      <c r="S6" s="1"/>
-      <c r="T6" s="1"/>
-      <c r="U6" s="1"/>
-      <c r="V6" s="1"/>
-      <c r="W6" s="1"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
+      <c r="R6" s="3"/>
+      <c r="S6" s="3"/>
+      <c r="T6" s="3"/>
+      <c r="U6" s="3"/>
+      <c r="V6" s="3"/>
+      <c r="W6" s="3"/>
     </row>
     <row r="7" ht="14.25" customHeight="1">
       <c r="A7" s="2" t="s">
@@ -626,10 +856,10 @@
       <c r="W7" s="1"/>
     </row>
     <row r="8" ht="14.25" customHeight="1">
-      <c r="A8" t="s">
+      <c r="A8" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="2" t="s">
         <v>17</v>
       </c>
       <c r="C8" s="2" t="s">
@@ -653,10 +883,10 @@
       <c r="W8" s="1"/>
     </row>
     <row r="9" ht="14.25" customHeight="1">
-      <c r="A9" s="2" t="s">
+      <c r="A9" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" t="s">
         <v>19</v>
       </c>
       <c r="C9" s="2" t="s">
@@ -775,17 +1005,17 @@
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
-      <c r="M13" s="3"/>
-      <c r="N13" s="3"/>
-      <c r="O13" s="3"/>
-      <c r="P13" s="3"/>
-      <c r="Q13" s="3"/>
-      <c r="R13" s="3"/>
-      <c r="S13" s="3"/>
-      <c r="T13" s="3"/>
-      <c r="U13" s="3"/>
-      <c r="V13" s="3"/>
-      <c r="W13" s="3"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+      <c r="Q13" s="1"/>
+      <c r="R13" s="1"/>
+      <c r="S13" s="1"/>
+      <c r="T13" s="1"/>
+      <c r="U13" s="1"/>
+      <c r="V13" s="1"/>
+      <c r="W13" s="1"/>
     </row>
     <row r="14" ht="14.25" customHeight="1">
       <c r="A14" s="2" t="s">
@@ -802,17 +1032,17 @@
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
-      <c r="M14" s="1"/>
-      <c r="N14" s="1"/>
-      <c r="O14" s="1"/>
-      <c r="P14" s="1"/>
-      <c r="Q14" s="1"/>
-      <c r="R14" s="1"/>
-      <c r="S14" s="1"/>
-      <c r="T14" s="1"/>
-      <c r="U14" s="1"/>
-      <c r="V14" s="1"/>
-      <c r="W14" s="1"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="3"/>
+      <c r="O14" s="3"/>
+      <c r="P14" s="3"/>
+      <c r="Q14" s="3"/>
+      <c r="R14" s="3"/>
+      <c r="S14" s="3"/>
+      <c r="T14" s="3"/>
+      <c r="U14" s="3"/>
+      <c r="V14" s="3"/>
+      <c r="W14" s="3"/>
     </row>
     <row r="15" ht="14.25" customHeight="1">
       <c r="A15" s="2" t="s">
@@ -842,10 +1072,10 @@
       <c r="W15" s="3"/>
     </row>
     <row r="16" ht="14.25" customHeight="1">
-      <c r="A16" t="s">
+      <c r="A16" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="2" t="s">
         <v>33</v>
       </c>
       <c r="C16" s="2" t="s">
@@ -856,24 +1086,24 @@
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
-      <c r="M16" s="1"/>
-      <c r="N16" s="1"/>
-      <c r="O16" s="1"/>
-      <c r="P16" s="1"/>
-      <c r="Q16" s="1"/>
-      <c r="R16" s="1"/>
-      <c r="S16" s="1"/>
-      <c r="T16" s="1"/>
-      <c r="U16" s="1"/>
-      <c r="V16" s="1"/>
-      <c r="W16" s="1"/>
+      <c r="M16" s="3"/>
+      <c r="N16" s="3"/>
+      <c r="O16" s="3"/>
+      <c r="P16" s="3"/>
+      <c r="Q16" s="3"/>
+      <c r="R16" s="3"/>
+      <c r="S16" s="3"/>
+      <c r="T16" s="3"/>
+      <c r="U16" s="3"/>
+      <c r="V16" s="3"/>
+      <c r="W16" s="3"/>
     </row>
     <row r="17" ht="14.25" customHeight="1">
       <c r="A17" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>5</v>
@@ -897,10 +1127,10 @@
     </row>
     <row r="18" ht="14.25" customHeight="1">
       <c r="A18" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>5</v>
@@ -910,24 +1140,24 @@
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
-      <c r="M18" s="1"/>
-      <c r="N18" s="1"/>
-      <c r="O18" s="1"/>
-      <c r="P18" s="1"/>
-      <c r="Q18" s="1"/>
-      <c r="R18" s="1"/>
-      <c r="S18" s="1"/>
-      <c r="T18" s="1"/>
-      <c r="U18" s="1"/>
-      <c r="V18" s="1"/>
-      <c r="W18" s="1"/>
+      <c r="M18" s="3"/>
+      <c r="N18" s="3"/>
+      <c r="O18" s="3"/>
+      <c r="P18" s="3"/>
+      <c r="Q18" s="3"/>
+      <c r="R18" s="3"/>
+      <c r="S18" s="3"/>
+      <c r="T18" s="3"/>
+      <c r="U18" s="3"/>
+      <c r="V18" s="3"/>
+      <c r="W18" s="3"/>
     </row>
     <row r="19" ht="14.25" customHeight="1">
-      <c r="A19" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>37</v>
+      <c r="A19" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" t="s">
+        <v>39</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>5</v>
@@ -1059,10 +1289,10 @@
     </row>
     <row r="24" ht="14.25" customHeight="1">
       <c r="A24" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>5</v>
@@ -1086,10 +1316,10 @@
     </row>
     <row r="25" ht="14.25" customHeight="1">
       <c r="A25" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>5</v>
@@ -1113,10 +1343,10 @@
     </row>
     <row r="26" ht="14.25" customHeight="1">
       <c r="A26" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>5</v>
@@ -1126,17 +1356,17 @@
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
       <c r="L26" s="1"/>
-      <c r="M26" s="3"/>
-      <c r="N26" s="3"/>
-      <c r="O26" s="3"/>
-      <c r="P26" s="3"/>
-      <c r="Q26" s="3"/>
-      <c r="R26" s="3"/>
-      <c r="S26" s="3"/>
-      <c r="T26" s="3"/>
-      <c r="U26" s="3"/>
-      <c r="V26" s="3"/>
-      <c r="W26" s="3"/>
+      <c r="M26" s="1"/>
+      <c r="N26" s="1"/>
+      <c r="O26" s="1"/>
+      <c r="P26" s="1"/>
+      <c r="Q26" s="1"/>
+      <c r="R26" s="1"/>
+      <c r="S26" s="1"/>
+      <c r="T26" s="1"/>
+      <c r="U26" s="1"/>
+      <c r="V26" s="1"/>
+      <c r="W26" s="1"/>
     </row>
     <row r="27" ht="14.25" customHeight="1">
       <c r="A27" s="2" t="s">
@@ -1166,10 +1396,10 @@
       <c r="W27" s="1"/>
     </row>
     <row r="28" ht="14.25" customHeight="1">
-      <c r="A28" t="s">
+      <c r="A28" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="2" t="s">
         <v>53</v>
       </c>
       <c r="C28" s="2" t="s">
@@ -1207,24 +1437,24 @@
       <c r="J29" s="1"/>
       <c r="K29" s="1"/>
       <c r="L29" s="1"/>
-      <c r="M29" s="1"/>
-      <c r="N29" s="1"/>
-      <c r="O29" s="1"/>
-      <c r="P29" s="1"/>
-      <c r="Q29" s="1"/>
-      <c r="R29" s="1"/>
-      <c r="S29" s="1"/>
-      <c r="T29" s="1"/>
-      <c r="U29" s="1"/>
-      <c r="V29" s="1"/>
-      <c r="W29" s="1"/>
+      <c r="M29" s="3"/>
+      <c r="N29" s="3"/>
+      <c r="O29" s="3"/>
+      <c r="P29" s="3"/>
+      <c r="Q29" s="3"/>
+      <c r="R29" s="3"/>
+      <c r="S29" s="3"/>
+      <c r="T29" s="3"/>
+      <c r="U29" s="3"/>
+      <c r="V29" s="3"/>
+      <c r="W29" s="3"/>
     </row>
     <row r="30" ht="14.25" customHeight="1">
       <c r="A30" s="2" t="s">
         <v>56</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>5</v>
@@ -1234,24 +1464,24 @@
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
       <c r="L30" s="1"/>
-      <c r="M30" s="1"/>
-      <c r="N30" s="1"/>
-      <c r="O30" s="1"/>
-      <c r="P30" s="1"/>
-      <c r="Q30" s="1"/>
-      <c r="R30" s="1"/>
-      <c r="S30" s="1"/>
-      <c r="T30" s="1"/>
-      <c r="U30" s="1"/>
-      <c r="V30" s="1"/>
-      <c r="W30" s="1"/>
+      <c r="M30" s="3"/>
+      <c r="N30" s="3"/>
+      <c r="O30" s="3"/>
+      <c r="P30" s="3"/>
+      <c r="Q30" s="3"/>
+      <c r="R30" s="3"/>
+      <c r="S30" s="3"/>
+      <c r="T30" s="3"/>
+      <c r="U30" s="3"/>
+      <c r="V30" s="3"/>
+      <c r="W30" s="3"/>
     </row>
     <row r="31" ht="14.25" customHeight="1">
       <c r="A31" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>5</v>
@@ -1275,10 +1505,10 @@
     </row>
     <row r="32" ht="14.25" customHeight="1">
       <c r="A32" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>5</v>
@@ -1288,24 +1518,24 @@
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
       <c r="L32" s="1"/>
-      <c r="M32" s="1"/>
-      <c r="N32" s="1"/>
-      <c r="O32" s="1"/>
-      <c r="P32" s="1"/>
-      <c r="Q32" s="1"/>
-      <c r="R32" s="1"/>
-      <c r="S32" s="1"/>
-      <c r="T32" s="1"/>
-      <c r="U32" s="1"/>
-      <c r="V32" s="1"/>
-      <c r="W32" s="1"/>
+      <c r="M32" s="3"/>
+      <c r="N32" s="3"/>
+      <c r="O32" s="3"/>
+      <c r="P32" s="3"/>
+      <c r="Q32" s="3"/>
+      <c r="R32" s="3"/>
+      <c r="S32" s="3"/>
+      <c r="T32" s="3"/>
+      <c r="U32" s="3"/>
+      <c r="V32" s="3"/>
+      <c r="W32" s="3"/>
     </row>
     <row r="33" ht="14.25" customHeight="1">
-      <c r="A33" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B33" s="2" t="s">
+      <c r="A33" t="s">
         <v>62</v>
+      </c>
+      <c r="B33" t="s">
+        <v>63</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>5</v>
@@ -1329,10 +1559,10 @@
     </row>
     <row r="34" ht="14.25" customHeight="1">
       <c r="A34" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>5</v>
@@ -1356,7 +1586,7 @@
     </row>
     <row r="35" ht="14.25" customHeight="1">
       <c r="A35" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>66</v>
@@ -1571,10 +1801,10 @@
       <c r="W42" s="1"/>
     </row>
     <row r="43" ht="14.25" customHeight="1">
-      <c r="A43" t="s">
+      <c r="A43" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43" s="2" t="s">
         <v>82</v>
       </c>
       <c r="C43" s="2" t="s">
@@ -1585,17 +1815,17 @@
       <c r="J43" s="1"/>
       <c r="K43" s="1"/>
       <c r="L43" s="1"/>
-      <c r="M43" s="1"/>
-      <c r="N43" s="1"/>
-      <c r="O43" s="1"/>
-      <c r="P43" s="1"/>
-      <c r="Q43" s="1"/>
-      <c r="R43" s="1"/>
-      <c r="S43" s="1"/>
-      <c r="T43" s="1"/>
-      <c r="U43" s="1"/>
-      <c r="V43" s="1"/>
-      <c r="W43" s="1"/>
+      <c r="M43" s="3"/>
+      <c r="N43" s="3"/>
+      <c r="O43" s="3"/>
+      <c r="P43" s="3"/>
+      <c r="Q43" s="3"/>
+      <c r="R43" s="3"/>
+      <c r="S43" s="3"/>
+      <c r="T43" s="3"/>
+      <c r="U43" s="3"/>
+      <c r="V43" s="3"/>
+      <c r="W43" s="3"/>
     </row>
     <row r="44" ht="14.25" customHeight="1">
       <c r="A44" s="2" t="s">
@@ -1706,7 +1936,7 @@
       <c r="W47" s="1"/>
     </row>
     <row r="48" ht="14.25" customHeight="1">
-      <c r="A48" t="s">
+      <c r="A48" s="2" t="s">
         <v>91</v>
       </c>
       <c r="B48" s="2" t="s">
@@ -1733,10 +1963,10 @@
       <c r="W48" s="1"/>
     </row>
     <row r="49" ht="14.25" customHeight="1">
-      <c r="A49" s="2" t="s">
+      <c r="A49" t="s">
         <v>93</v>
       </c>
-      <c r="B49" s="2" t="s">
+      <c r="B49" t="s">
         <v>94</v>
       </c>
       <c r="C49" s="2" t="s">
@@ -1855,17 +2085,17 @@
       <c r="J53" s="1"/>
       <c r="K53" s="1"/>
       <c r="L53" s="1"/>
-      <c r="M53" s="3"/>
-      <c r="N53" s="3"/>
-      <c r="O53" s="3"/>
-      <c r="P53" s="3"/>
-      <c r="Q53" s="3"/>
-      <c r="R53" s="3"/>
-      <c r="S53" s="3"/>
-      <c r="T53" s="3"/>
-      <c r="U53" s="3"/>
-      <c r="V53" s="3"/>
-      <c r="W53" s="3"/>
+      <c r="M53" s="1"/>
+      <c r="N53" s="1"/>
+      <c r="O53" s="1"/>
+      <c r="P53" s="1"/>
+      <c r="Q53" s="1"/>
+      <c r="R53" s="1"/>
+      <c r="S53" s="1"/>
+      <c r="T53" s="1"/>
+      <c r="U53" s="1"/>
+      <c r="V53" s="1"/>
+      <c r="W53" s="1"/>
     </row>
     <row r="54" ht="14.25" customHeight="1">
       <c r="A54" s="2" t="s">
@@ -1882,20 +2112,20 @@
       <c r="J54" s="1"/>
       <c r="K54" s="1"/>
       <c r="L54" s="1"/>
-      <c r="M54" s="3"/>
-      <c r="N54" s="3"/>
-      <c r="O54" s="3"/>
-      <c r="P54" s="3"/>
-      <c r="Q54" s="3"/>
-      <c r="R54" s="3"/>
-      <c r="S54" s="3"/>
-      <c r="T54" s="3"/>
-      <c r="U54" s="3"/>
-      <c r="V54" s="3"/>
-      <c r="W54" s="3"/>
+      <c r="M54" s="1"/>
+      <c r="N54" s="1"/>
+      <c r="O54" s="1"/>
+      <c r="P54" s="1"/>
+      <c r="Q54" s="1"/>
+      <c r="R54" s="1"/>
+      <c r="S54" s="1"/>
+      <c r="T54" s="1"/>
+      <c r="U54" s="1"/>
+      <c r="V54" s="1"/>
+      <c r="W54" s="1"/>
     </row>
     <row r="55" ht="14.25" customHeight="1">
-      <c r="A55" s="2" t="s">
+      <c r="A55" t="s">
         <v>105</v>
       </c>
       <c r="B55" s="2" t="s">
@@ -1909,17 +2139,17 @@
       <c r="J55" s="1"/>
       <c r="K55" s="1"/>
       <c r="L55" s="1"/>
-      <c r="M55" s="3"/>
-      <c r="N55" s="3"/>
-      <c r="O55" s="3"/>
-      <c r="P55" s="3"/>
-      <c r="Q55" s="3"/>
-      <c r="R55" s="3"/>
-      <c r="S55" s="3"/>
-      <c r="T55" s="3"/>
-      <c r="U55" s="3"/>
-      <c r="V55" s="3"/>
-      <c r="W55" s="3"/>
+      <c r="M55" s="1"/>
+      <c r="N55" s="1"/>
+      <c r="O55" s="1"/>
+      <c r="P55" s="1"/>
+      <c r="Q55" s="1"/>
+      <c r="R55" s="1"/>
+      <c r="S55" s="1"/>
+      <c r="T55" s="1"/>
+      <c r="U55" s="1"/>
+      <c r="V55" s="1"/>
+      <c r="W55" s="1"/>
     </row>
     <row r="56" ht="14.25" customHeight="1">
       <c r="A56" s="2" t="s">
@@ -1963,17 +2193,17 @@
       <c r="J57" s="1"/>
       <c r="K57" s="1"/>
       <c r="L57" s="1"/>
-      <c r="M57" s="3"/>
-      <c r="N57" s="3"/>
-      <c r="O57" s="3"/>
-      <c r="P57" s="3"/>
-      <c r="Q57" s="3"/>
-      <c r="R57" s="3"/>
-      <c r="S57" s="3"/>
-      <c r="T57" s="3"/>
-      <c r="U57" s="3"/>
-      <c r="V57" s="3"/>
-      <c r="W57" s="3"/>
+      <c r="M57" s="1"/>
+      <c r="N57" s="1"/>
+      <c r="O57" s="1"/>
+      <c r="P57" s="1"/>
+      <c r="Q57" s="1"/>
+      <c r="R57" s="1"/>
+      <c r="S57" s="1"/>
+      <c r="T57" s="1"/>
+      <c r="U57" s="1"/>
+      <c r="V57" s="1"/>
+      <c r="W57" s="1"/>
     </row>
     <row r="58" ht="14.25" customHeight="1">
       <c r="A58" s="2" t="s">
@@ -1990,17 +2220,17 @@
       <c r="J58" s="1"/>
       <c r="K58" s="1"/>
       <c r="L58" s="1"/>
-      <c r="M58" s="3"/>
-      <c r="N58" s="3"/>
-      <c r="O58" s="3"/>
-      <c r="P58" s="3"/>
-      <c r="Q58" s="3"/>
-      <c r="R58" s="3"/>
-      <c r="S58" s="3"/>
-      <c r="T58" s="3"/>
-      <c r="U58" s="3"/>
-      <c r="V58" s="3"/>
-      <c r="W58" s="3"/>
+      <c r="M58" s="1"/>
+      <c r="N58" s="1"/>
+      <c r="O58" s="1"/>
+      <c r="P58" s="1"/>
+      <c r="Q58" s="1"/>
+      <c r="R58" s="1"/>
+      <c r="S58" s="1"/>
+      <c r="T58" s="1"/>
+      <c r="U58" s="1"/>
+      <c r="V58" s="1"/>
+      <c r="W58" s="1"/>
     </row>
     <row r="59" ht="14.25" customHeight="1">
       <c r="A59" s="2" t="s">
@@ -2044,19 +2274,28 @@
       <c r="J60" s="1"/>
       <c r="K60" s="1"/>
       <c r="L60" s="1"/>
-      <c r="M60" s="3"/>
-      <c r="N60" s="3"/>
-      <c r="O60" s="3"/>
-      <c r="P60" s="3"/>
-      <c r="Q60" s="3"/>
-      <c r="R60" s="3"/>
-      <c r="S60" s="3"/>
-      <c r="T60" s="3"/>
-      <c r="U60" s="3"/>
-      <c r="V60" s="3"/>
-      <c r="W60" s="3"/>
+      <c r="M60" s="1"/>
+      <c r="N60" s="1"/>
+      <c r="O60" s="1"/>
+      <c r="P60" s="1"/>
+      <c r="Q60" s="1"/>
+      <c r="R60" s="1"/>
+      <c r="S60" s="1"/>
+      <c r="T60" s="1"/>
+      <c r="U60" s="1"/>
+      <c r="V60" s="1"/>
+      <c r="W60" s="1"/>
     </row>
     <row r="61" ht="14.25" customHeight="1">
+      <c r="A61" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="H61" s="1"/>
       <c r="I61" s="1"/>
       <c r="J61" s="1"/>
@@ -2075,6 +2314,15 @@
       <c r="W61" s="3"/>
     </row>
     <row r="62" ht="14.25" customHeight="1">
+      <c r="A62" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="H62" s="1"/>
       <c r="I62" s="1"/>
       <c r="J62" s="1"/>
@@ -2093,6 +2341,15 @@
       <c r="W62" s="3"/>
     </row>
     <row r="63" ht="14.25" customHeight="1">
+      <c r="A63" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="H63" s="1"/>
       <c r="I63" s="1"/>
       <c r="J63" s="1"/>
@@ -2111,6 +2368,15 @@
       <c r="W63" s="3"/>
     </row>
     <row r="64" ht="14.25" customHeight="1">
+      <c r="A64" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="H64" s="1"/>
       <c r="I64" s="1"/>
       <c r="J64" s="1"/>
@@ -2129,6 +2395,15 @@
       <c r="W64" s="3"/>
     </row>
     <row r="65" ht="14.25" customHeight="1">
+      <c r="A65" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="H65" s="1"/>
       <c r="I65" s="1"/>
       <c r="J65" s="1"/>
@@ -2147,6 +2422,15 @@
       <c r="W65" s="3"/>
     </row>
     <row r="66" ht="14.25" customHeight="1">
+      <c r="A66" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="H66" s="1"/>
       <c r="I66" s="1"/>
       <c r="J66" s="1"/>
@@ -2165,6 +2449,15 @@
       <c r="W66" s="3"/>
     </row>
     <row r="67" ht="14.25" customHeight="1">
+      <c r="A67" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="H67" s="1"/>
       <c r="I67" s="1"/>
       <c r="J67" s="1"/>
@@ -2183,6 +2476,15 @@
       <c r="W67" s="3"/>
     </row>
     <row r="68" ht="14.25" customHeight="1">
+      <c r="A68" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="H68" s="1"/>
       <c r="I68" s="1"/>
       <c r="J68" s="1"/>
@@ -2201,6 +2503,15 @@
       <c r="W68" s="3"/>
     </row>
     <row r="69" ht="14.25" customHeight="1">
+      <c r="A69" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="H69" s="1"/>
       <c r="I69" s="1"/>
       <c r="J69" s="1"/>
@@ -2219,6 +2530,15 @@
       <c r="W69" s="3"/>
     </row>
     <row r="70" ht="14.25" customHeight="1">
+      <c r="A70" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="H70" s="1"/>
       <c r="I70" s="1"/>
       <c r="J70" s="1"/>
@@ -2237,6 +2557,15 @@
       <c r="W70" s="3"/>
     </row>
     <row r="71" ht="14.25" customHeight="1">
+      <c r="A71" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="H71" s="1"/>
       <c r="I71" s="1"/>
       <c r="J71" s="1"/>
@@ -2255,6 +2584,15 @@
       <c r="W71" s="3"/>
     </row>
     <row r="72" ht="14.25" customHeight="1">
+      <c r="A72" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>141</v>
+      </c>
       <c r="H72" s="1"/>
       <c r="I72" s="1"/>
       <c r="J72" s="1"/>
@@ -2273,6 +2611,15 @@
       <c r="W72" s="3"/>
     </row>
     <row r="73" ht="14.25" customHeight="1">
+      <c r="A73" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="H73" s="1"/>
       <c r="I73" s="1"/>
       <c r="J73" s="1"/>
@@ -2291,6 +2638,15 @@
       <c r="W73" s="3"/>
     </row>
     <row r="74" ht="14.25" customHeight="1">
+      <c r="A74" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="H74" s="1"/>
       <c r="I74" s="1"/>
       <c r="J74" s="1"/>
@@ -2309,6 +2665,15 @@
       <c r="W74" s="3"/>
     </row>
     <row r="75" ht="14.25" customHeight="1">
+      <c r="A75" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="H75" s="1"/>
       <c r="I75" s="1"/>
       <c r="J75" s="1"/>
@@ -2327,6 +2692,15 @@
       <c r="W75" s="3"/>
     </row>
     <row r="76" ht="14.25" customHeight="1">
+      <c r="A76" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="H76" s="1"/>
       <c r="I76" s="1"/>
       <c r="J76" s="1"/>
@@ -2345,6 +2719,15 @@
       <c r="W76" s="3"/>
     </row>
     <row r="77" ht="14.25" customHeight="1">
+      <c r="A77" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="H77" s="1"/>
       <c r="I77" s="1"/>
       <c r="J77" s="1"/>
@@ -2363,6 +2746,15 @@
       <c r="W77" s="3"/>
     </row>
     <row r="78" ht="14.25" customHeight="1">
+      <c r="A78" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>153</v>
+      </c>
       <c r="H78" s="1"/>
       <c r="I78" s="1"/>
       <c r="J78" s="1"/>
@@ -2381,6 +2773,15 @@
       <c r="W78" s="3"/>
     </row>
     <row r="79" ht="14.25" customHeight="1">
+      <c r="A79" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="C79" s="4" t="s">
+        <v>155</v>
+      </c>
       <c r="H79" s="1"/>
       <c r="I79" s="1"/>
       <c r="J79" s="1"/>
@@ -2399,6 +2800,15 @@
       <c r="W79" s="3"/>
     </row>
     <row r="80" ht="14.25" customHeight="1">
+      <c r="A80" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>158</v>
+      </c>
       <c r="H80" s="1"/>
       <c r="I80" s="1"/>
       <c r="J80" s="1"/>
@@ -2417,6 +2827,15 @@
       <c r="W80" s="3"/>
     </row>
     <row r="81" ht="14.25" customHeight="1">
+      <c r="A81" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="H81" s="1"/>
       <c r="I81" s="1"/>
       <c r="J81" s="1"/>
@@ -2435,6 +2854,15 @@
       <c r="W81" s="3"/>
     </row>
     <row r="82" ht="14.25" customHeight="1">
+      <c r="A82" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>141</v>
+      </c>
       <c r="H82" s="1"/>
       <c r="I82" s="1"/>
       <c r="J82" s="1"/>
@@ -2453,6 +2881,15 @@
       <c r="W82" s="3"/>
     </row>
     <row r="83" ht="14.25" customHeight="1">
+      <c r="A83" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="H83" s="1"/>
       <c r="I83" s="1"/>
       <c r="J83" s="1"/>
@@ -2471,6 +2908,15 @@
       <c r="W83" s="3"/>
     </row>
     <row r="84" ht="14.25" customHeight="1">
+      <c r="A84" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="C84" s="2">
+        <v>1.0</v>
+      </c>
       <c r="H84" s="1"/>
       <c r="I84" s="1"/>
       <c r="J84" s="1"/>
@@ -2489,6 +2935,15 @@
       <c r="W84" s="3"/>
     </row>
     <row r="85" ht="14.25" customHeight="1">
+      <c r="A85" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="C85" s="2">
+        <v>2.0</v>
+      </c>
       <c r="H85" s="1"/>
       <c r="I85" s="1"/>
       <c r="J85" s="1"/>
@@ -2507,6 +2962,15 @@
       <c r="W85" s="3"/>
     </row>
     <row r="86" ht="14.25" customHeight="1">
+      <c r="A86" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="C86" s="2">
+        <v>3.0</v>
+      </c>
       <c r="H86" s="1"/>
       <c r="I86" s="1"/>
       <c r="J86" s="1"/>
@@ -2525,6 +2989,15 @@
       <c r="W86" s="3"/>
     </row>
     <row r="87" ht="14.25" customHeight="1">
+      <c r="A87" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="C87" s="2">
+        <v>4.0</v>
+      </c>
       <c r="H87" s="1"/>
       <c r="I87" s="1"/>
       <c r="J87" s="1"/>
@@ -2543,6 +3016,15 @@
       <c r="W87" s="3"/>
     </row>
     <row r="88" ht="14.25" customHeight="1">
+      <c r="A88" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C88" s="2">
+        <v>5.0</v>
+      </c>
       <c r="H88" s="1"/>
       <c r="I88" s="1"/>
       <c r="J88" s="1"/>
@@ -2561,6 +3043,15 @@
       <c r="W88" s="3"/>
     </row>
     <row r="89" ht="14.25" customHeight="1">
+      <c r="A89" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="C89" s="2">
+        <v>6.0</v>
+      </c>
       <c r="H89" s="1"/>
       <c r="I89" s="1"/>
       <c r="J89" s="1"/>
@@ -2579,6 +3070,15 @@
       <c r="W89" s="3"/>
     </row>
     <row r="90" ht="14.25" customHeight="1">
+      <c r="A90" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="C90" s="2">
+        <v>7.0</v>
+      </c>
       <c r="H90" s="1"/>
       <c r="I90" s="1"/>
       <c r="J90" s="1"/>
@@ -2597,6 +3097,15 @@
       <c r="W90" s="3"/>
     </row>
     <row r="91" ht="14.25" customHeight="1">
+      <c r="A91" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C91" s="2">
+        <v>8.0</v>
+      </c>
       <c r="H91" s="1"/>
       <c r="I91" s="1"/>
       <c r="J91" s="1"/>
@@ -2615,6 +3124,15 @@
       <c r="W91" s="3"/>
     </row>
     <row r="92" ht="14.25" customHeight="1">
+      <c r="A92" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="C92" s="2">
+        <v>9.0</v>
+      </c>
       <c r="H92" s="1"/>
       <c r="I92" s="1"/>
       <c r="J92" s="1"/>
@@ -2633,6 +3151,15 @@
       <c r="W92" s="3"/>
     </row>
     <row r="93" ht="14.25" customHeight="1">
+      <c r="A93" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="C93" s="2">
+        <v>10.0</v>
+      </c>
       <c r="H93" s="1"/>
       <c r="I93" s="1"/>
       <c r="J93" s="1"/>
@@ -2651,6 +3178,15 @@
       <c r="W93" s="3"/>
     </row>
     <row r="94" ht="14.25" customHeight="1">
+      <c r="A94" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="C94" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="H94" s="1"/>
       <c r="I94" s="1"/>
       <c r="J94" s="1"/>
@@ -2669,6 +3205,15 @@
       <c r="W94" s="3"/>
     </row>
     <row r="95" ht="14.25" customHeight="1">
+      <c r="A95" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>189</v>
+      </c>
       <c r="H95" s="1"/>
       <c r="I95" s="1"/>
       <c r="J95" s="1"/>

</xml_diff>

<commit_message>
New background for localization. Fixes for post-race events. UI created for post-race events with two NPCs, with this feature now properly supported by the Simulation.
</commit_message>
<xml_diff>
--- a/stm-unity/Assets/Localization/Sports Team Manager Localization.xlsx
+++ b/stm-unity/Assets/Localization/Sports Team Manager Localization.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="208">
   <si>
     <t>key</t>
   </si>
@@ -272,6 +272,12 @@
   </si>
   <si>
     <t>Mood</t>
+  </si>
+  <si>
+    <t>MY_CREW</t>
+  </si>
+  <si>
+    <t>My Crew</t>
   </si>
   <si>
     <t>NAME</t>
@@ -1920,17 +1926,17 @@
       <c r="J45" s="2"/>
       <c r="K45" s="2"/>
       <c r="L45" s="2"/>
-      <c r="M45" s="2"/>
-      <c r="N45" s="2"/>
-      <c r="O45" s="2"/>
-      <c r="P45" s="2"/>
-      <c r="Q45" s="2"/>
-      <c r="R45" s="2"/>
-      <c r="S45" s="2"/>
-      <c r="T45" s="2"/>
-      <c r="U45" s="2"/>
-      <c r="V45" s="2"/>
-      <c r="W45" s="2"/>
+      <c r="M45" s="1"/>
+      <c r="N45" s="1"/>
+      <c r="O45" s="1"/>
+      <c r="P45" s="1"/>
+      <c r="Q45" s="1"/>
+      <c r="R45" s="1"/>
+      <c r="S45" s="1"/>
+      <c r="T45" s="1"/>
+      <c r="U45" s="1"/>
+      <c r="V45" s="1"/>
+      <c r="W45" s="1"/>
     </row>
     <row r="46" ht="14.25" customHeight="1">
       <c r="A46" s="3" t="s">
@@ -1947,17 +1953,17 @@
       <c r="J46" s="2"/>
       <c r="K46" s="2"/>
       <c r="L46" s="2"/>
-      <c r="M46" s="1"/>
-      <c r="N46" s="1"/>
-      <c r="O46" s="1"/>
-      <c r="P46" s="1"/>
-      <c r="Q46" s="1"/>
-      <c r="R46" s="1"/>
-      <c r="S46" s="1"/>
-      <c r="T46" s="1"/>
-      <c r="U46" s="1"/>
-      <c r="V46" s="1"/>
-      <c r="W46" s="1"/>
+      <c r="M46" s="2"/>
+      <c r="N46" s="2"/>
+      <c r="O46" s="2"/>
+      <c r="P46" s="2"/>
+      <c r="Q46" s="2"/>
+      <c r="R46" s="2"/>
+      <c r="S46" s="2"/>
+      <c r="T46" s="2"/>
+      <c r="U46" s="2"/>
+      <c r="V46" s="2"/>
+      <c r="W46" s="2"/>
     </row>
     <row r="47" ht="14.25" customHeight="1">
       <c r="A47" s="3" t="s">
@@ -1987,10 +1993,10 @@
       <c r="W47" s="1"/>
     </row>
     <row r="48" ht="14.25" customHeight="1">
-      <c r="A48" t="s">
+      <c r="A48" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="B48" s="4" t="s">
         <v>94</v>
       </c>
       <c r="C48" s="3" t="s">
@@ -2001,23 +2007,23 @@
       <c r="J48" s="2"/>
       <c r="K48" s="2"/>
       <c r="L48" s="2"/>
-      <c r="M48" s="2"/>
-      <c r="N48" s="2"/>
-      <c r="O48" s="2"/>
-      <c r="P48" s="2"/>
-      <c r="Q48" s="2"/>
-      <c r="R48" s="2"/>
-      <c r="S48" s="2"/>
-      <c r="T48" s="2"/>
-      <c r="U48" s="2"/>
-      <c r="V48" s="2"/>
-      <c r="W48" s="2"/>
+      <c r="M48" s="1"/>
+      <c r="N48" s="1"/>
+      <c r="O48" s="1"/>
+      <c r="P48" s="1"/>
+      <c r="Q48" s="1"/>
+      <c r="R48" s="1"/>
+      <c r="S48" s="1"/>
+      <c r="T48" s="1"/>
+      <c r="U48" s="1"/>
+      <c r="V48" s="1"/>
+      <c r="W48" s="1"/>
     </row>
     <row r="49" ht="14.25" customHeight="1">
-      <c r="A49" s="3" t="s">
+      <c r="A49" t="s">
         <v>95</v>
       </c>
-      <c r="B49" s="4" t="s">
+      <c r="B49" s="1" t="s">
         <v>96</v>
       </c>
       <c r="C49" s="3" t="s">
@@ -2028,17 +2034,17 @@
       <c r="J49" s="2"/>
       <c r="K49" s="2"/>
       <c r="L49" s="2"/>
-      <c r="M49" s="1"/>
-      <c r="N49" s="1"/>
-      <c r="O49" s="1"/>
-      <c r="P49" s="1"/>
-      <c r="Q49" s="1"/>
-      <c r="R49" s="1"/>
-      <c r="S49" s="1"/>
-      <c r="T49" s="1"/>
-      <c r="U49" s="1"/>
-      <c r="V49" s="1"/>
-      <c r="W49" s="1"/>
+      <c r="M49" s="2"/>
+      <c r="N49" s="2"/>
+      <c r="O49" s="2"/>
+      <c r="P49" s="2"/>
+      <c r="Q49" s="2"/>
+      <c r="R49" s="2"/>
+      <c r="S49" s="2"/>
+      <c r="T49" s="2"/>
+      <c r="U49" s="2"/>
+      <c r="V49" s="2"/>
+      <c r="W49" s="2"/>
     </row>
     <row r="50" ht="14.25" customHeight="1">
       <c r="A50" s="3" t="s">
@@ -2082,17 +2088,17 @@
       <c r="J51" s="2"/>
       <c r="K51" s="2"/>
       <c r="L51" s="2"/>
-      <c r="M51" s="2"/>
-      <c r="N51" s="2"/>
-      <c r="O51" s="2"/>
-      <c r="P51" s="2"/>
-      <c r="Q51" s="2"/>
-      <c r="R51" s="2"/>
-      <c r="S51" s="2"/>
-      <c r="T51" s="2"/>
-      <c r="U51" s="2"/>
-      <c r="V51" s="2"/>
-      <c r="W51" s="2"/>
+      <c r="M51" s="1"/>
+      <c r="N51" s="1"/>
+      <c r="O51" s="1"/>
+      <c r="P51" s="1"/>
+      <c r="Q51" s="1"/>
+      <c r="R51" s="1"/>
+      <c r="S51" s="1"/>
+      <c r="T51" s="1"/>
+      <c r="U51" s="1"/>
+      <c r="V51" s="1"/>
+      <c r="W51" s="1"/>
     </row>
     <row r="52" ht="14.25" customHeight="1">
       <c r="A52" s="3" t="s">
@@ -2109,24 +2115,24 @@
       <c r="J52" s="2"/>
       <c r="K52" s="2"/>
       <c r="L52" s="2"/>
-      <c r="M52" s="1"/>
-      <c r="N52" s="1"/>
-      <c r="O52" s="1"/>
-      <c r="P52" s="1"/>
-      <c r="Q52" s="1"/>
-      <c r="R52" s="1"/>
-      <c r="S52" s="1"/>
-      <c r="T52" s="1"/>
-      <c r="U52" s="1"/>
-      <c r="V52" s="1"/>
-      <c r="W52" s="1"/>
+      <c r="M52" s="2"/>
+      <c r="N52" s="2"/>
+      <c r="O52" s="2"/>
+      <c r="P52" s="2"/>
+      <c r="Q52" s="2"/>
+      <c r="R52" s="2"/>
+      <c r="S52" s="2"/>
+      <c r="T52" s="2"/>
+      <c r="U52" s="2"/>
+      <c r="V52" s="2"/>
+      <c r="W52" s="2"/>
     </row>
     <row r="53" ht="14.25" customHeight="1">
       <c r="A53" s="3" t="s">
         <v>103</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C53" s="3" t="s">
         <v>5</v>
@@ -2136,21 +2142,21 @@
       <c r="J53" s="2"/>
       <c r="K53" s="2"/>
       <c r="L53" s="2"/>
-      <c r="M53" s="2"/>
-      <c r="N53" s="2"/>
-      <c r="O53" s="2"/>
-      <c r="P53" s="2"/>
-      <c r="Q53" s="2"/>
-      <c r="R53" s="2"/>
-      <c r="S53" s="2"/>
-      <c r="T53" s="2"/>
-      <c r="U53" s="2"/>
-      <c r="V53" s="2"/>
-      <c r="W53" s="2"/>
+      <c r="M53" s="1"/>
+      <c r="N53" s="1"/>
+      <c r="O53" s="1"/>
+      <c r="P53" s="1"/>
+      <c r="Q53" s="1"/>
+      <c r="R53" s="1"/>
+      <c r="S53" s="1"/>
+      <c r="T53" s="1"/>
+      <c r="U53" s="1"/>
+      <c r="V53" s="1"/>
+      <c r="W53" s="1"/>
     </row>
     <row r="54" ht="14.25" customHeight="1">
       <c r="A54" s="3" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B54" s="4" t="s">
         <v>105</v>
@@ -2163,17 +2169,17 @@
       <c r="J54" s="2"/>
       <c r="K54" s="2"/>
       <c r="L54" s="2"/>
-      <c r="M54" s="1"/>
-      <c r="N54" s="1"/>
-      <c r="O54" s="1"/>
-      <c r="P54" s="1"/>
-      <c r="Q54" s="1"/>
-      <c r="R54" s="1"/>
-      <c r="S54" s="1"/>
-      <c r="T54" s="1"/>
-      <c r="U54" s="1"/>
-      <c r="V54" s="1"/>
-      <c r="W54" s="1"/>
+      <c r="M54" s="2"/>
+      <c r="N54" s="2"/>
+      <c r="O54" s="2"/>
+      <c r="P54" s="2"/>
+      <c r="Q54" s="2"/>
+      <c r="R54" s="2"/>
+      <c r="S54" s="2"/>
+      <c r="T54" s="2"/>
+      <c r="U54" s="2"/>
+      <c r="V54" s="2"/>
+      <c r="W54" s="2"/>
     </row>
     <row r="55" ht="14.25" customHeight="1">
       <c r="A55" s="3" t="s">
@@ -2190,17 +2196,17 @@
       <c r="J55" s="2"/>
       <c r="K55" s="2"/>
       <c r="L55" s="2"/>
-      <c r="M55" s="2"/>
-      <c r="N55" s="2"/>
-      <c r="O55" s="2"/>
-      <c r="P55" s="2"/>
-      <c r="Q55" s="2"/>
-      <c r="R55" s="2"/>
-      <c r="S55" s="2"/>
-      <c r="T55" s="2"/>
-      <c r="U55" s="2"/>
-      <c r="V55" s="2"/>
-      <c r="W55" s="2"/>
+      <c r="M55" s="1"/>
+      <c r="N55" s="1"/>
+      <c r="O55" s="1"/>
+      <c r="P55" s="1"/>
+      <c r="Q55" s="1"/>
+      <c r="R55" s="1"/>
+      <c r="S55" s="1"/>
+      <c r="T55" s="1"/>
+      <c r="U55" s="1"/>
+      <c r="V55" s="1"/>
+      <c r="W55" s="1"/>
     </row>
     <row r="56" ht="14.25" customHeight="1">
       <c r="A56" s="3" t="s">
@@ -2217,17 +2223,17 @@
       <c r="J56" s="2"/>
       <c r="K56" s="2"/>
       <c r="L56" s="2"/>
-      <c r="M56" s="1"/>
-      <c r="N56" s="1"/>
-      <c r="O56" s="1"/>
-      <c r="P56" s="1"/>
-      <c r="Q56" s="1"/>
-      <c r="R56" s="1"/>
-      <c r="S56" s="1"/>
-      <c r="T56" s="1"/>
-      <c r="U56" s="1"/>
-      <c r="V56" s="1"/>
-      <c r="W56" s="1"/>
+      <c r="M56" s="2"/>
+      <c r="N56" s="2"/>
+      <c r="O56" s="2"/>
+      <c r="P56" s="2"/>
+      <c r="Q56" s="2"/>
+      <c r="R56" s="2"/>
+      <c r="S56" s="2"/>
+      <c r="T56" s="2"/>
+      <c r="U56" s="2"/>
+      <c r="V56" s="2"/>
+      <c r="W56" s="2"/>
     </row>
     <row r="57" ht="14.25" customHeight="1">
       <c r="A57" s="3" t="s">
@@ -2263,8 +2269,8 @@
       <c r="B58" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="C58" s="3">
-        <v>1.0</v>
+      <c r="C58" s="3" t="s">
+        <v>5</v>
       </c>
       <c r="H58" s="2"/>
       <c r="I58" s="2"/>
@@ -2291,7 +2297,7 @@
         <v>115</v>
       </c>
       <c r="C59" s="3">
-        <v>10.0</v>
+        <v>1.0</v>
       </c>
       <c r="H59" s="2"/>
       <c r="I59" s="2"/>
@@ -2318,7 +2324,7 @@
         <v>117</v>
       </c>
       <c r="C60" s="3">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="H60" s="2"/>
       <c r="I60" s="2"/>
@@ -2345,7 +2351,7 @@
         <v>119</v>
       </c>
       <c r="C61" s="3">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="H61" s="2"/>
       <c r="I61" s="2"/>
@@ -2372,7 +2378,7 @@
         <v>121</v>
       </c>
       <c r="C62" s="3">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="H62" s="2"/>
       <c r="I62" s="2"/>
@@ -2399,7 +2405,7 @@
         <v>123</v>
       </c>
       <c r="C63" s="3">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
       <c r="H63" s="2"/>
       <c r="I63" s="2"/>
@@ -2426,7 +2432,7 @@
         <v>125</v>
       </c>
       <c r="C64" s="3">
-        <v>6.0</v>
+        <v>5.0</v>
       </c>
       <c r="H64" s="2"/>
       <c r="I64" s="2"/>
@@ -2453,7 +2459,7 @@
         <v>127</v>
       </c>
       <c r="C65" s="3">
-        <v>7.0</v>
+        <v>6.0</v>
       </c>
       <c r="H65" s="2"/>
       <c r="I65" s="2"/>
@@ -2480,7 +2486,7 @@
         <v>129</v>
       </c>
       <c r="C66" s="3">
-        <v>8.0</v>
+        <v>7.0</v>
       </c>
       <c r="H66" s="2"/>
       <c r="I66" s="2"/>
@@ -2507,7 +2513,7 @@
         <v>131</v>
       </c>
       <c r="C67" s="3">
-        <v>9.0</v>
+        <v>8.0</v>
       </c>
       <c r="H67" s="2"/>
       <c r="I67" s="2"/>
@@ -2533,25 +2539,25 @@
       <c r="B68" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="C68" s="3" t="s">
-        <v>5</v>
+      <c r="C68" s="3">
+        <v>9.0</v>
       </c>
       <c r="H68" s="2"/>
       <c r="I68" s="2"/>
       <c r="J68" s="2"/>
       <c r="K68" s="2"/>
       <c r="L68" s="2"/>
-      <c r="M68" s="2"/>
-      <c r="N68" s="2"/>
-      <c r="O68" s="2"/>
-      <c r="P68" s="2"/>
-      <c r="Q68" s="2"/>
-      <c r="R68" s="2"/>
-      <c r="S68" s="2"/>
-      <c r="T68" s="2"/>
-      <c r="U68" s="2"/>
-      <c r="V68" s="2"/>
-      <c r="W68" s="2"/>
+      <c r="M68" s="1"/>
+      <c r="N68" s="1"/>
+      <c r="O68" s="1"/>
+      <c r="P68" s="1"/>
+      <c r="Q68" s="1"/>
+      <c r="R68" s="1"/>
+      <c r="S68" s="1"/>
+      <c r="T68" s="1"/>
+      <c r="U68" s="1"/>
+      <c r="V68" s="1"/>
+      <c r="W68" s="1"/>
     </row>
     <row r="69" ht="14.25" customHeight="1">
       <c r="A69" s="3" t="s">
@@ -2615,34 +2621,34 @@
         <v>139</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>140</v>
+        <v>5</v>
       </c>
       <c r="H71" s="2"/>
       <c r="I71" s="2"/>
       <c r="J71" s="2"/>
       <c r="K71" s="2"/>
       <c r="L71" s="2"/>
-      <c r="M71" s="1"/>
-      <c r="N71" s="1"/>
-      <c r="O71" s="1"/>
-      <c r="P71" s="1"/>
-      <c r="Q71" s="1"/>
-      <c r="R71" s="1"/>
-      <c r="S71" s="1"/>
-      <c r="T71" s="1"/>
-      <c r="U71" s="1"/>
-      <c r="V71" s="1"/>
-      <c r="W71" s="1"/>
+      <c r="M71" s="2"/>
+      <c r="N71" s="2"/>
+      <c r="O71" s="2"/>
+      <c r="P71" s="2"/>
+      <c r="Q71" s="2"/>
+      <c r="R71" s="2"/>
+      <c r="S71" s="2"/>
+      <c r="T71" s="2"/>
+      <c r="U71" s="2"/>
+      <c r="V71" s="2"/>
+      <c r="W71" s="2"/>
     </row>
     <row r="72" ht="14.25" customHeight="1">
       <c r="A72" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="B72" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="B72" s="4" t="s">
+      <c r="C72" s="3" t="s">
         <v>142</v>
-      </c>
-      <c r="C72" s="3" t="s">
-        <v>5</v>
       </c>
       <c r="H72" s="2"/>
       <c r="I72" s="2"/>
@@ -2669,7 +2675,7 @@
         <v>144</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>54</v>
+        <v>5</v>
       </c>
       <c r="H73" s="2"/>
       <c r="I73" s="2"/>
@@ -2696,7 +2702,7 @@
         <v>146</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>5</v>
+        <v>54</v>
       </c>
       <c r="H74" s="2"/>
       <c r="I74" s="2"/>
@@ -2750,7 +2756,7 @@
         <v>150</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>151</v>
+        <v>5</v>
       </c>
       <c r="H76" s="2"/>
       <c r="I76" s="2"/>
@@ -2771,30 +2777,30 @@
     </row>
     <row r="77" ht="14.25" customHeight="1">
       <c r="A77" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="B77" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="B77" s="4" t="s">
+      <c r="C77" s="3" t="s">
         <v>153</v>
-      </c>
-      <c r="C77" s="3" t="s">
-        <v>5</v>
       </c>
       <c r="H77" s="2"/>
       <c r="I77" s="2"/>
       <c r="J77" s="2"/>
       <c r="K77" s="2"/>
       <c r="L77" s="2"/>
-      <c r="M77" s="2"/>
-      <c r="N77" s="2"/>
-      <c r="O77" s="2"/>
-      <c r="P77" s="2"/>
-      <c r="Q77" s="2"/>
-      <c r="R77" s="2"/>
-      <c r="S77" s="2"/>
-      <c r="T77" s="2"/>
-      <c r="U77" s="2"/>
-      <c r="V77" s="2"/>
-      <c r="W77" s="2"/>
+      <c r="M77" s="1"/>
+      <c r="N77" s="1"/>
+      <c r="O77" s="1"/>
+      <c r="P77" s="1"/>
+      <c r="Q77" s="1"/>
+      <c r="R77" s="1"/>
+      <c r="S77" s="1"/>
+      <c r="T77" s="1"/>
+      <c r="U77" s="1"/>
+      <c r="V77" s="1"/>
+      <c r="W77" s="1"/>
     </row>
     <row r="78" ht="14.25" customHeight="1">
       <c r="A78" s="3" t="s">
@@ -2811,20 +2817,20 @@
       <c r="J78" s="2"/>
       <c r="K78" s="2"/>
       <c r="L78" s="2"/>
-      <c r="M78" s="1"/>
-      <c r="N78" s="1"/>
-      <c r="O78" s="1"/>
-      <c r="P78" s="1"/>
-      <c r="Q78" s="1"/>
-      <c r="R78" s="1"/>
-      <c r="S78" s="1"/>
-      <c r="T78" s="1"/>
-      <c r="U78" s="1"/>
-      <c r="V78" s="1"/>
-      <c r="W78" s="1"/>
+      <c r="M78" s="2"/>
+      <c r="N78" s="2"/>
+      <c r="O78" s="2"/>
+      <c r="P78" s="2"/>
+      <c r="Q78" s="2"/>
+      <c r="R78" s="2"/>
+      <c r="S78" s="2"/>
+      <c r="T78" s="2"/>
+      <c r="U78" s="2"/>
+      <c r="V78" s="2"/>
+      <c r="W78" s="2"/>
     </row>
     <row r="79" ht="14.25" customHeight="1">
-      <c r="A79" s="5" t="s">
+      <c r="A79" s="3" t="s">
         <v>156</v>
       </c>
       <c r="B79" s="4" t="s">
@@ -2905,7 +2911,7 @@
       <c r="W81" s="1"/>
     </row>
     <row r="82" ht="14.25" customHeight="1">
-      <c r="A82" s="3" t="s">
+      <c r="A82" s="5" t="s">
         <v>162</v>
       </c>
       <c r="B82" s="4" t="s">
@@ -2919,17 +2925,17 @@
       <c r="J82" s="2"/>
       <c r="K82" s="2"/>
       <c r="L82" s="2"/>
-      <c r="M82" s="2"/>
-      <c r="N82" s="2"/>
-      <c r="O82" s="2"/>
-      <c r="P82" s="2"/>
-      <c r="Q82" s="2"/>
-      <c r="R82" s="2"/>
-      <c r="S82" s="2"/>
-      <c r="T82" s="2"/>
-      <c r="U82" s="2"/>
-      <c r="V82" s="2"/>
-      <c r="W82" s="2"/>
+      <c r="M82" s="1"/>
+      <c r="N82" s="1"/>
+      <c r="O82" s="1"/>
+      <c r="P82" s="1"/>
+      <c r="Q82" s="1"/>
+      <c r="R82" s="1"/>
+      <c r="S82" s="1"/>
+      <c r="T82" s="1"/>
+      <c r="U82" s="1"/>
+      <c r="V82" s="1"/>
+      <c r="W82" s="1"/>
     </row>
     <row r="83" ht="14.25" customHeight="1">
       <c r="A83" s="3" t="s">
@@ -2946,17 +2952,17 @@
       <c r="J83" s="2"/>
       <c r="K83" s="2"/>
       <c r="L83" s="2"/>
-      <c r="M83" s="1"/>
-      <c r="N83" s="1"/>
-      <c r="O83" s="1"/>
-      <c r="P83" s="1"/>
-      <c r="Q83" s="1"/>
-      <c r="R83" s="1"/>
-      <c r="S83" s="1"/>
-      <c r="T83" s="1"/>
-      <c r="U83" s="1"/>
-      <c r="V83" s="1"/>
-      <c r="W83" s="1"/>
+      <c r="M83" s="2"/>
+      <c r="N83" s="2"/>
+      <c r="O83" s="2"/>
+      <c r="P83" s="2"/>
+      <c r="Q83" s="2"/>
+      <c r="R83" s="2"/>
+      <c r="S83" s="2"/>
+      <c r="T83" s="2"/>
+      <c r="U83" s="2"/>
+      <c r="V83" s="2"/>
+      <c r="W83" s="2"/>
     </row>
     <row r="84" ht="14.25" customHeight="1">
       <c r="A84" s="3" t="s">
@@ -3000,17 +3006,17 @@
       <c r="J85" s="2"/>
       <c r="K85" s="2"/>
       <c r="L85" s="2"/>
-      <c r="M85" s="2"/>
-      <c r="N85" s="2"/>
-      <c r="O85" s="2"/>
-      <c r="P85" s="2"/>
-      <c r="Q85" s="2"/>
-      <c r="R85" s="2"/>
-      <c r="S85" s="2"/>
-      <c r="T85" s="2"/>
-      <c r="U85" s="2"/>
-      <c r="V85" s="2"/>
-      <c r="W85" s="2"/>
+      <c r="M85" s="1"/>
+      <c r="N85" s="1"/>
+      <c r="O85" s="1"/>
+      <c r="P85" s="1"/>
+      <c r="Q85" s="1"/>
+      <c r="R85" s="1"/>
+      <c r="S85" s="1"/>
+      <c r="T85" s="1"/>
+      <c r="U85" s="1"/>
+      <c r="V85" s="1"/>
+      <c r="W85" s="1"/>
     </row>
     <row r="86" ht="14.25" customHeight="1">
       <c r="A86" s="3" t="s">
@@ -3121,10 +3127,10 @@
       <c r="W89" s="2"/>
     </row>
     <row r="90" ht="14.25" customHeight="1">
-      <c r="A90" t="s">
+      <c r="A90" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="B90" s="1" t="s">
+      <c r="B90" s="4" t="s">
         <v>179</v>
       </c>
       <c r="C90" s="3" t="s">
@@ -3148,10 +3154,10 @@
       <c r="W90" s="2"/>
     </row>
     <row r="91" ht="14.25" customHeight="1">
-      <c r="A91" s="3" t="s">
+      <c r="A91" t="s">
         <v>180</v>
       </c>
-      <c r="B91" s="4" t="s">
+      <c r="B91" s="1" t="s">
         <v>181</v>
       </c>
       <c r="C91" s="3" t="s">
@@ -3189,17 +3195,17 @@
       <c r="J92" s="2"/>
       <c r="K92" s="2"/>
       <c r="L92" s="2"/>
-      <c r="M92" s="1"/>
-      <c r="N92" s="1"/>
-      <c r="O92" s="1"/>
-      <c r="P92" s="1"/>
-      <c r="Q92" s="1"/>
-      <c r="R92" s="1"/>
-      <c r="S92" s="1"/>
-      <c r="T92" s="1"/>
-      <c r="U92" s="1"/>
-      <c r="V92" s="1"/>
-      <c r="W92" s="1"/>
+      <c r="M92" s="2"/>
+      <c r="N92" s="2"/>
+      <c r="O92" s="2"/>
+      <c r="P92" s="2"/>
+      <c r="Q92" s="2"/>
+      <c r="R92" s="2"/>
+      <c r="S92" s="2"/>
+      <c r="T92" s="2"/>
+      <c r="U92" s="2"/>
+      <c r="V92" s="2"/>
+      <c r="W92" s="2"/>
     </row>
     <row r="93" ht="14.25" customHeight="1">
       <c r="A93" s="3" t="s">
@@ -3243,17 +3249,17 @@
       <c r="J94" s="2"/>
       <c r="K94" s="2"/>
       <c r="L94" s="2"/>
-      <c r="M94" s="2"/>
-      <c r="N94" s="2"/>
-      <c r="O94" s="2"/>
-      <c r="P94" s="2"/>
-      <c r="Q94" s="2"/>
-      <c r="R94" s="2"/>
-      <c r="S94" s="2"/>
-      <c r="T94" s="2"/>
-      <c r="U94" s="2"/>
-      <c r="V94" s="2"/>
-      <c r="W94" s="2"/>
+      <c r="M94" s="1"/>
+      <c r="N94" s="1"/>
+      <c r="O94" s="1"/>
+      <c r="P94" s="1"/>
+      <c r="Q94" s="1"/>
+      <c r="R94" s="1"/>
+      <c r="S94" s="1"/>
+      <c r="T94" s="1"/>
+      <c r="U94" s="1"/>
+      <c r="V94" s="1"/>
+      <c r="W94" s="1"/>
     </row>
     <row r="95" ht="14.25" customHeight="1">
       <c r="A95" s="3" t="s">
@@ -3310,7 +3316,7 @@
       <c r="W96" s="2"/>
     </row>
     <row r="97" ht="14.25" customHeight="1">
-      <c r="A97" t="s">
+      <c r="A97" s="3" t="s">
         <v>192</v>
       </c>
       <c r="B97" s="4" t="s">
@@ -3337,7 +3343,7 @@
       <c r="W97" s="2"/>
     </row>
     <row r="98" ht="14.25" customHeight="1">
-      <c r="A98" s="3" t="s">
+      <c r="A98" t="s">
         <v>194</v>
       </c>
       <c r="B98" s="4" t="s">
@@ -3351,17 +3357,17 @@
       <c r="J98" s="2"/>
       <c r="K98" s="2"/>
       <c r="L98" s="2"/>
-      <c r="M98" s="1"/>
-      <c r="N98" s="1"/>
-      <c r="O98" s="1"/>
-      <c r="P98" s="1"/>
-      <c r="Q98" s="1"/>
-      <c r="R98" s="1"/>
-      <c r="S98" s="1"/>
-      <c r="T98" s="1"/>
-      <c r="U98" s="1"/>
-      <c r="V98" s="1"/>
-      <c r="W98" s="1"/>
+      <c r="M98" s="2"/>
+      <c r="N98" s="2"/>
+      <c r="O98" s="2"/>
+      <c r="P98" s="2"/>
+      <c r="Q98" s="2"/>
+      <c r="R98" s="2"/>
+      <c r="S98" s="2"/>
+      <c r="T98" s="2"/>
+      <c r="U98" s="2"/>
+      <c r="V98" s="2"/>
+      <c r="W98" s="2"/>
     </row>
     <row r="99" ht="14.25" customHeight="1">
       <c r="A99" s="3" t="s">
@@ -3405,17 +3411,17 @@
       <c r="J100" s="2"/>
       <c r="K100" s="2"/>
       <c r="L100" s="2"/>
-      <c r="M100" s="2"/>
-      <c r="N100" s="2"/>
-      <c r="O100" s="2"/>
-      <c r="P100" s="2"/>
-      <c r="Q100" s="2"/>
-      <c r="R100" s="2"/>
-      <c r="S100" s="2"/>
-      <c r="T100" s="2"/>
-      <c r="U100" s="2"/>
-      <c r="V100" s="2"/>
-      <c r="W100" s="2"/>
+      <c r="M100" s="1"/>
+      <c r="N100" s="1"/>
+      <c r="O100" s="1"/>
+      <c r="P100" s="1"/>
+      <c r="Q100" s="1"/>
+      <c r="R100" s="1"/>
+      <c r="S100" s="1"/>
+      <c r="T100" s="1"/>
+      <c r="U100" s="1"/>
+      <c r="V100" s="1"/>
+      <c r="W100" s="1"/>
     </row>
     <row r="101" ht="14.25" customHeight="1">
       <c r="A101" s="3" t="s">
@@ -3459,17 +3465,17 @@
       <c r="J102" s="2"/>
       <c r="K102" s="2"/>
       <c r="L102" s="2"/>
-      <c r="M102" s="1"/>
-      <c r="N102" s="1"/>
-      <c r="O102" s="1"/>
-      <c r="P102" s="1"/>
-      <c r="Q102" s="1"/>
-      <c r="R102" s="1"/>
-      <c r="S102" s="1"/>
-      <c r="T102" s="1"/>
-      <c r="U102" s="1"/>
-      <c r="V102" s="1"/>
-      <c r="W102" s="1"/>
+      <c r="M102" s="2"/>
+      <c r="N102" s="2"/>
+      <c r="O102" s="2"/>
+      <c r="P102" s="2"/>
+      <c r="Q102" s="2"/>
+      <c r="R102" s="2"/>
+      <c r="S102" s="2"/>
+      <c r="T102" s="2"/>
+      <c r="U102" s="2"/>
+      <c r="V102" s="2"/>
+      <c r="W102" s="2"/>
     </row>
     <row r="103" ht="14.25" customHeight="1">
       <c r="A103" s="3" t="s">
@@ -3486,37 +3492,44 @@
       <c r="J103" s="2"/>
       <c r="K103" s="2"/>
       <c r="L103" s="2"/>
-      <c r="M103" s="2"/>
-      <c r="N103" s="2"/>
-      <c r="O103" s="2"/>
-      <c r="P103" s="2"/>
-      <c r="Q103" s="2"/>
-      <c r="R103" s="2"/>
-      <c r="S103" s="2"/>
-      <c r="T103" s="2"/>
-      <c r="U103" s="2"/>
-      <c r="V103" s="2"/>
-      <c r="W103" s="2"/>
+      <c r="M103" s="1"/>
+      <c r="N103" s="1"/>
+      <c r="O103" s="1"/>
+      <c r="P103" s="1"/>
+      <c r="Q103" s="1"/>
+      <c r="R103" s="1"/>
+      <c r="S103" s="1"/>
+      <c r="T103" s="1"/>
+      <c r="U103" s="1"/>
+      <c r="V103" s="1"/>
+      <c r="W103" s="1"/>
     </row>
     <row r="104" ht="14.25" customHeight="1">
-      <c r="B104" s="1"/>
-      <c r="C104" s="3"/>
+      <c r="A104" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="B104" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="C104" s="3" t="s">
+        <v>5</v>
+      </c>
       <c r="H104" s="2"/>
       <c r="I104" s="2"/>
       <c r="J104" s="2"/>
       <c r="K104" s="2"/>
       <c r="L104" s="2"/>
-      <c r="M104" s="1"/>
-      <c r="N104" s="1"/>
-      <c r="O104" s="1"/>
-      <c r="P104" s="1"/>
-      <c r="Q104" s="1"/>
-      <c r="R104" s="1"/>
-      <c r="S104" s="1"/>
-      <c r="T104" s="1"/>
-      <c r="U104" s="1"/>
-      <c r="V104" s="1"/>
-      <c r="W104" s="1"/>
+      <c r="M104" s="2"/>
+      <c r="N104" s="2"/>
+      <c r="O104" s="2"/>
+      <c r="P104" s="2"/>
+      <c r="Q104" s="2"/>
+      <c r="R104" s="2"/>
+      <c r="S104" s="2"/>
+      <c r="T104" s="2"/>
+      <c r="U104" s="2"/>
+      <c r="V104" s="2"/>
+      <c r="W104" s="2"/>
     </row>
     <row r="105" ht="14.25" customHeight="1">
       <c r="B105" s="1"/>

</xml_diff>

<commit_message>
Slight change to decay and mood calculations in EA file. Settings pop-up set up for UI. TODO: Change language in all UI on change, settings pop-up whilst playing.
</commit_message>
<xml_diff>
--- a/stm-unity/Assets/Localization/Sports Team Manager Localization.xlsx
+++ b/stm-unity/Assets/Localization/Sports Team Manager Localization.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="218">
   <si>
     <t>key</t>
   </si>
@@ -638,6 +638,36 @@
   <si>
     <t>Yes</t>
   </si>
+  <si>
+    <t>MUSIC</t>
+  </si>
+  <si>
+    <t>Music</t>
+  </si>
+  <si>
+    <t>SOUND</t>
+  </si>
+  <si>
+    <t>Sound FX</t>
+  </si>
+  <si>
+    <t>LANGUAGE</t>
+  </si>
+  <si>
+    <t>Language</t>
+  </si>
+  <si>
+    <t>ENGLISH</t>
+  </si>
+  <si>
+    <t>English</t>
+  </si>
+  <si>
+    <t>ITALIAN</t>
+  </si>
+  <si>
+    <t>Italian</t>
+  </si>
 </sst>
 </file>
 
@@ -3532,7 +3562,15 @@
       <c r="W104" s="2"/>
     </row>
     <row r="105" ht="14.25" customHeight="1">
-      <c r="B105" s="1"/>
+      <c r="A105" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="B105" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="C105" s="3" t="s">
+        <v>5</v>
+      </c>
       <c r="H105" s="2"/>
       <c r="I105" s="2"/>
       <c r="J105" s="2"/>
@@ -3551,7 +3589,15 @@
       <c r="W105" s="1"/>
     </row>
     <row r="106" ht="14.25" customHeight="1">
-      <c r="B106" s="1"/>
+      <c r="A106" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="B106" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="C106" s="3" t="s">
+        <v>5</v>
+      </c>
       <c r="H106" s="2"/>
       <c r="I106" s="2"/>
       <c r="J106" s="2"/>
@@ -3570,7 +3616,15 @@
       <c r="W106" s="1"/>
     </row>
     <row r="107" ht="14.25" customHeight="1">
-      <c r="B107" s="1"/>
+      <c r="A107" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="B107" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="C107" s="3" t="s">
+        <v>5</v>
+      </c>
       <c r="H107" s="2"/>
       <c r="I107" s="2"/>
       <c r="J107" s="2"/>
@@ -3589,7 +3643,15 @@
       <c r="W107" s="1"/>
     </row>
     <row r="108" ht="14.25" customHeight="1">
-      <c r="B108" s="1"/>
+      <c r="A108" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="B108" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="C108" s="3" t="s">
+        <v>5</v>
+      </c>
       <c r="H108" s="2"/>
       <c r="I108" s="2"/>
       <c r="J108" s="2"/>
@@ -3608,7 +3670,15 @@
       <c r="W108" s="1"/>
     </row>
     <row r="109" ht="14.25" customHeight="1">
-      <c r="B109" s="1"/>
+      <c r="A109" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="B109" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="C109" s="3" t="s">
+        <v>5</v>
+      </c>
       <c r="H109" s="2"/>
       <c r="I109" s="2"/>
       <c r="J109" s="2"/>
@@ -3627,7 +3697,15 @@
       <c r="W109" s="1"/>
     </row>
     <row r="110" ht="14.25" customHeight="1">
-      <c r="B110" s="1"/>
+      <c r="A110" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="B110" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="C110" s="3" t="s">
+        <v>5</v>
+      </c>
       <c r="H110" s="2"/>
       <c r="I110" s="2"/>
       <c r="J110" s="2"/>

</xml_diff>